<commit_message>
fixed referral mappings and modified proguress course schema
</commit_message>
<xml_diff>
--- a/mapping/mml4_summary_mapping.xlsx
+++ b/mapping/mml4_summary_mapping.xlsx
@@ -2998,10 +2998,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/content[openEHR-EHR-SECTION.summary_outline.v1]/items[at0010]/items[openEHR-EHR-INSTRUCTION.medication_order.v0]/activities[at0001]/description[at0002]/items[at0070]//mappings/target/code_string</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>/content[openEHR-EHR-SECTION.summary_outline.v1]/items[at0010]/items[openEHR-EHR-INSTRUCTION.medication_order.v0]/activities[at0001]/description[at0002]/items[at0070]/mappings/target/terminology_id/value</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -3055,6 +3051,10 @@
   </si>
   <si>
     <t>/content[openEHR-EHR-SECTION.summary_outline.v1]/items[at0010]/items[openEHR-EHR-INSTRUCTION.medication_order.v0]/activities[at0001]/description[at0002]/items[at0044]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.summary_outline.v1]/items[at0010]/items[openEHR-EHR-INSTRUCTION.medication_order.v0]/activities[at0001]/description[at0002]/items[at0070]/mappings/target/code_string</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3653,7 +3653,7 @@
   <dimension ref="A1:N700"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A323" workbookViewId="0">
-      <selection activeCell="A351" sqref="A351:K351"/>
+      <selection activeCell="K336" sqref="K336"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -10940,7 +10940,7 @@
       </c>
       <c r="F335" s="29"/>
       <c r="K335" s="12" t="s">
-        <v>786</v>
+        <v>800</v>
       </c>
       <c r="L335" s="12"/>
     </row>
@@ -10958,7 +10958,7 @@
       </c>
       <c r="F336" s="29"/>
       <c r="K336" s="12" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="L336" s="12"/>
     </row>
@@ -10973,7 +10973,7 @@
         <v>730</v>
       </c>
       <c r="K337" s="12" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="L337" s="12"/>
     </row>
@@ -10997,7 +10997,7 @@
         <v>734</v>
       </c>
       <c r="K338" s="12" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="L338" s="12"/>
     </row>
@@ -11015,7 +11015,7 @@
       <c r="E339" s="29"/>
       <c r="F339" s="29"/>
       <c r="K339" s="12" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="L339" s="12"/>
     </row>
@@ -11039,7 +11039,7 @@
         <v>734</v>
       </c>
       <c r="K340" s="12" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="L340" s="12"/>
     </row>
@@ -11065,7 +11065,7 @@
         <v>740</v>
       </c>
       <c r="K341" s="12" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="L341" s="12"/>
     </row>
@@ -11091,7 +11091,7 @@
         <v>743</v>
       </c>
       <c r="K342" s="12" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="L342" s="12"/>
     </row>
@@ -11117,7 +11117,7 @@
         <v>723</v>
       </c>
       <c r="K343" s="12" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="L343" s="12"/>
     </row>
@@ -11143,7 +11143,7 @@
         <v>748</v>
       </c>
       <c r="K344" s="12" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="L344" s="12"/>
     </row>
@@ -11169,7 +11169,7 @@
         <v>723</v>
       </c>
       <c r="K345" s="12" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="L345" s="12"/>
     </row>
@@ -11195,7 +11195,7 @@
         <v>723</v>
       </c>
       <c r="K346" s="12" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="L346" s="12"/>
     </row>
@@ -11221,7 +11221,7 @@
         <v>755</v>
       </c>
       <c r="K347" s="12" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="L347" s="12"/>
     </row>
@@ -11247,7 +11247,7 @@
         <v>748</v>
       </c>
       <c r="K348" s="12" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="L348" s="12"/>
     </row>
@@ -11295,7 +11295,7 @@
         <v>723</v>
       </c>
       <c r="K350" s="12" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="L350" s="12"/>
     </row>

</xml_diff>

<commit_message>
fixed summary table mapping, table of testMemo in report module
</commit_message>
<xml_diff>
--- a/mapping/mml4_summary_mapping.xlsx
+++ b/mapping/mml4_summary_mapping.xlsx
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2053" uniqueCount="908">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2054" uniqueCount="909">
   <si>
     <t>Elements　</t>
   </si>
@@ -3123,12 +3123,16 @@
     <t>Point in Time2</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>*</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3205,6 +3209,14 @@
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
@@ -3375,7 +3387,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3593,6 +3605,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3912,7 +3927,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N378"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A253" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E267" sqref="E267"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -10033,7 +10050,9 @@
       </c>
       <c r="C282" s="8"/>
       <c r="D282" s="8"/>
-      <c r="E282" s="8"/>
+      <c r="E282" s="73" t="s">
+        <v>908</v>
+      </c>
       <c r="F282" s="8"/>
       <c r="H282" s="2" t="s">
         <v>487</v>
@@ -12101,6 +12120,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="I6" location="Sheet2!$B$38" display="start date/time"/>
     <hyperlink ref="I7" location="Sheet2!$B$48" display="end date/time"/>
@@ -12340,28 +12364,5 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="notEqual" id="{92B60613-0501-4EA8-8553-11682C114713}">
-            <xm:f>#REF!</xm:f>
-            <x14:dxf>
-              <font>
-                <b/>
-                <i/>
-              </font>
-              <fill>
-                <patternFill patternType="none">
-                  <bgColor auto="1"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>A1:XFD1048576</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>